<commit_message>
Refactor Lab 3: realistic bash simulation and CSV backend
</commit_message>
<xml_diff>
--- a/dpu simulator/doca_installation_commands.xlsx
+++ b/dpu simulator/doca_installation_commands.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DOCA Installation" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,24 +27,14 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0076933C"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -65,16 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,19 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="5" customWidth="1" min="1" max="1"/>
-    <col width="65" customWidth="1" min="2" max="2"/>
-    <col width="80" customWidth="1" min="3" max="3"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -473,15 +451,15 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>sudo –i</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>[sudo] password for student:
 Sorry, try again.
@@ -491,41 +469,41 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>cd /home/student/AI_Infra/module5/hands_on_1</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>/usr/sbin/ofed_uninstall.sh --force</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>bash: /usr/sbin/ofed_uninstall.sh: No such file or directory</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>sudo apt-get autoremove</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Reading package lists... Done
 Building dependency tree... Done
@@ -535,82 +513,89 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>dpkg -i doca-host_3.1.0-091000-25.07-ubuntu2204_amd64.deb</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>dpkg: error: requested operation requires superuser privilege</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>sudo -i</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>root@acad14:~#</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>for f in $( dpkg --list | grep doca | awk '{print $2}' ); do echo $f ; apt remove --purge $f -y ; done</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>doca-host
+(Reading database ... 194224 files and directories currently installed.)
+Removing doca-host (3.1.0-091000-25.07-ubuntu2204) ...
+Purging configuration files for doca-host (3.1.0-091000-25.07-ubuntu2204) ...</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>/usr/sbin/ofed_uninstall.sh --force</t>
         </is>
       </c>
-      <c r="C9" s="3" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>-bash: /usr/sbin/ofed_uninstall.sh: No such file or directory</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>cd /home/student/AI_Infra/module5/hands_on_1</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>dpkg -i doca-host_3.1.0-091000-25.07-ubuntu2204_amd64.deb</t>
         </is>
       </c>
-      <c r="C11" s="3" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Selecting previously unselected package doca-host.
 (Reading database ... 194224 files and directories currently installed.)
@@ -621,15 +606,15 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>apt update</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Fetched 21.9 MB in 4s (6,219 kB/s)
 Reading package lists... Done
@@ -640,65 +625,71 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>systemctl status rshim</t>
         </is>
       </c>
-      <c r="C13" s="3" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Unit rshim.service could not be found.</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>apt install rshim</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>apt install -y rshim</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>Reading package lists... Done
+Building dependency tree... Done
+Reading state information... Done
 The following NEW packages will be installed:
   rshim
 0 upgraded, 1 newly installed, 0 to remove and 347 not upgraded.
-Unpacking rshim (2.4.4-0.g4a0b69d.2507097) ...
-Setting up rshim (2.4.4-0.g4a0b69d.2507097) ...
-Installation complete. To enable and start the rshim service, run:
-  systemctl daemon-reload
-  systemctl enable rshim
-  systemctl start rshim</t>
+Need to get 14.2 kB of archives.
+After this operation, 45.1 kB of additional disk space will be used.
+Get:1 http://archive.ubuntu.com/ubuntu jammy/main amd64 rshim amd64 2.0.6-0ubuntu1 [14.2 kB]
+Fetched 14.2 kB in 0s (35.6 kB/s)
+Selecting previously unselected package rshim.
+(Reading database ... 194224 files and directories currently installed.)
+Preparing to unpack .../rshim_2.0.6-0ubuntu1_amd64.deb ...
+Unpacking rshim (2.0.6-0ubuntu1) ...
+Setting up rshim (2.0.6-0ubuntu1) ...
+Created symlink /etc/systemd/system/multi-user.target.wants/rshim.service → /lib/systemd/system/rshim.service.</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>sudo systemctl start rshim</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>apt install -y doca-all mlnx-fw-updater</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>21 upgraded, 160 newly installed, 7 to remove and 325 not upgraded.
 Need to get 14.0 MB/416 MB of archives.
@@ -715,71 +706,71 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>exit</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>logout</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>sudo minicom -D /dev/rshim0/console</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>minicom: cannot open /dev/rshim0/console: No such file or directory</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>sudo systemctl start rshim</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>sudo minicom -D /dev/rshim0/console</t>
         </is>
       </c>
-      <c r="C20" s="3" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>minicom: cannot open /dev/rshim0/console: No such file or directory</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>sudo systemctl status rshim</t>
         </is>
       </c>
-      <c r="C21" s="3" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>● rshim.service - rshim driver for BlueField SoC
      Active: active (running) since Sun 2025-11-23 07:28:43 PST
@@ -792,37 +783,37 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>sudo systemctl stop rshim</t>
         </is>
       </c>
-      <c r="C22" s="3" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>sudo systemctl start rshim</t>
         </is>
       </c>
-      <c r="C23" s="3" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>sudo minicom -D /dev/rshim0/console</t>
         </is>
       </c>
-      <c r="C24" s="3" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Welcome to minicom 2.8
 Port /dev/rshim0/console, 07:33:52
@@ -832,83 +823,46 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="inlineStr">
-        <is>
-          <t>[DPU] ubuntu</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="inlineStr">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ubuntu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>Password:</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="inlineStr">
-        <is>
-          <t>[DPU] (password entered)</t>
-        </is>
-      </c>
-      <c r="C26" s="3" t="inlineStr">
-        <is>
-          <t>You are required to change your password immediately (administrator enforced).
-Changing password for ubuntu.
-Current password:</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="inlineStr">
-        <is>
-          <t>[DPU] (new passwords entered)</t>
-        </is>
-      </c>
-      <c r="C27" s="3" t="inlineStr">
-        <is>
-          <t>Welcome to Ubuntu 22.04.5 LTS (GNU/Linux 5.15.0-1056-bluefield aarch64)
-  System load:  0.01               Temperature:               75.0 C
-  Usage of /:   4.1% of 116.76GB   Processes:                 299
-  Memory usage: 4%                 Users logged in:           0
-  Swap usage:   0%                 IPv4 address for oob_net0: 10.184.212.164
-ubuntu@acad14-DPU:~$</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A26" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="inlineStr">
-        <is>
-          <t>[DPU] sudo -i</t>
-        </is>
-      </c>
-      <c r="C28" s="3" t="inlineStr">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>sudo -i</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>sudo: unable to resolve host acad14-DPU: Temporary failure in name resolution
 root@acad14-DPU:~#</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
+    <row r="27">
+      <c r="A27" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="inlineStr">
-        <is>
-          <t>[DPU] sudo bfver</t>
-        </is>
-      </c>
-      <c r="C29" s="3" t="inlineStr">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>sudo bfver</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
         <is>
           <t>--/dev/mmcblk0boot0
 BlueField ATF version: v2.2(release):4.9.0-25-g0ce57e322

</xml_diff>